<commit_message>
Mise en place des questionnaires
AJout des questions pour les 2 questionnaires
</commit_message>
<xml_diff>
--- a/Questionaire_Hellink.xlsx
+++ b/Questionaire_Hellink.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ADF10B-D006-4DEE-A6DD-BB36366356D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,9 +19,75 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Questionnaire de Playtest Hellink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informations global </t>
+  </si>
+  <si>
+    <t>Nom (optinel)</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Genre 
+(Homme/Femme)</t>
+  </si>
+  <si>
+    <t>Information liées aux jeux vidéo</t>
+  </si>
+  <si>
+    <t>Fréquence 
+de jeu</t>
+  </si>
+  <si>
+    <t>Genre de 
+jeu préféré</t>
+  </si>
+  <si>
+    <t>Jeu préféré</t>
+  </si>
+  <si>
+    <t>Plateforme de jeu préféré (pc,ps4,xbox one…)</t>
+  </si>
+  <si>
+    <t>Fréquence d'utilisation de internet</t>
+  </si>
+  <si>
+    <t>Informations utile 
+par rapport au jeu testé</t>
+  </si>
+  <si>
+    <t>Information par rapport au test</t>
+  </si>
+  <si>
+    <t>Noté votre amusement durant le test sur une échelle de 1 à 5 (5 positif, 1 négatif)</t>
+  </si>
+  <si>
+    <t>Noté votre facilité à utilisé le jeu (commande) sur une échelle de 1 à 5 (5 positif, 1 négatif)</t>
+  </si>
+  <si>
+    <t>Avez-vous lu tout le textes, un partie ou pas lu le texte</t>
+  </si>
+  <si>
+    <t>D'après vous que voulai mettre en avant Hellink</t>
+  </si>
+  <si>
+    <t>Sur une échelle de 1 à 5 avez-vous appris des choses (5 positif, 1 négatif)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +95,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -45,12 +137,264 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +674,262 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" customWidth="1"/>
+    <col min="13" max="15" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="27"/>
+    </row>
+    <row r="4" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="K3:O3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rajout d'espace de commentaire
Ajout d'espace de commentaire dans les deux questionnaires
</commit_message>
<xml_diff>
--- a/Questionaire_Hellink.xlsx
+++ b/Questionaire_Hellink.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ADF10B-D006-4DEE-A6DD-BB36366356D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9066CB24-996C-4C49-8091-0F29D2FFE5F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="21">
   <si>
     <t>Questionnaire de Playtest Hellink</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Sur une échelle de 1 à 5 avez-vous appris des choses (5 positif, 1 négatif)</t>
+  </si>
+  <si>
+    <t>écriver vos commentaires :</t>
+  </si>
+  <si>
+    <t>écrivez vos commentaires :</t>
   </si>
 </sst>
 </file>
@@ -103,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +134,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -321,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -335,6 +347,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,15 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -362,21 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,14 +407,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,11 +714,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,70 +736,70 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="17" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="23" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="27"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="30"/>
     </row>
     <row r="4" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="21" t="s">
         <v>18</v>
       </c>
     </row>
@@ -924,11 +963,192 @@
       <c r="N14" s="7"/>
       <c r="O14" s="8"/>
     </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="32"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="33"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="32"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="33"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="32"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="33"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="33"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="33"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="33"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="33"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="32"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="K3:O3"/>
+    <mergeCell ref="B16:O16"/>
+    <mergeCell ref="B17:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>